<commit_message>
added regression section and plotted results
</commit_message>
<xml_diff>
--- a/Project2/Data/lakedata.xlsx
+++ b/Project2/Data/lakedata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/087f5d83ccd9606c/Desktop/GitRepos/Deeplearning-Workshops-FYP/Project2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yassy\OneDrive\Desktop\GitRepos\Deeplearning-Workshops-FYP\Project2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{BE4F0EF6-B4A1-43AA-AD29-FFB8C4AFB82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBBB1F32-37CA-45E3-86DD-EE3B37DEC851}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4E6A9A-6F87-4F87-BED2-FF922B1C3FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15840" xr2:uid="{31151B04-E7BF-49C0-B722-C4434B4119E4}"/>
   </bookViews>
@@ -33,6 +33,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Data</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,267 +391,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8C3644-AF7E-463F-9804-0B5333E4C46B}">
-  <dimension ref="A1:A98"/>
+  <dimension ref="A1:A99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A98"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>10.38</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>11.86</v>
+        <v>10.38</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>10.97</v>
+        <v>11.86</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>10.8</v>
+        <v>10.97</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>9.7899999999999991</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>10.39</v>
+        <v>9.7899999999999991</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>10.42</v>
+        <v>10.39</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>10.82</v>
+        <v>10.42</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>11.4</v>
+        <v>10.82</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>11.32</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>11.44</v>
+        <v>11.32</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11.68</v>
+        <v>11.44</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11.17</v>
+        <v>11.68</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>10.53</v>
+        <v>11.17</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>10.01</v>
+        <v>10.53</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>9.91</v>
+        <v>10.01</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>9.14</v>
+        <v>9.91</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>9.16</v>
+        <v>9.14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>9.5500000000000007</v>
+        <v>9.16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>9.67</v>
+        <v>9.5500000000000007</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
+        <v>9.67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>8.44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>8.24</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>9.1</v>
+        <v>8.24</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>9.09</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9.35</v>
+        <v>9.09</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>8.82</v>
+        <v>9.35</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>9.32</v>
+        <v>8.82</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>9.01</v>
+        <v>9.32</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>9</v>
+        <v>9.01</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>9.8000000000000007</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>9.83</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>9.7200000000000006</v>
+        <v>9.83</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>9.89</v>
+        <v>9.7200000000000006</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>10.01</v>
+        <v>9.89</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>9.3699999999999992</v>
+        <v>10.01</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>8.69</v>
+        <v>9.3699999999999992</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>8.19</v>
+        <v>8.69</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>8.67</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>9.5500000000000007</v>
+        <v>8.67</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>8.92</v>
+        <v>9.5500000000000007</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>8.09</v>
+        <v>8.92</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>9.3699999999999992</v>
+        <v>8.09</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>10.130000000000001</v>
+        <v>9.3699999999999992</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>10.14</v>
+        <v>10.130000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>9.51</v>
+        <v>10.14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>9.24</v>
+        <v>9.51</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>8.66</v>
+        <v>9.24</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>8.86</v>
+        <v>8.66</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>8.0500000000000007</v>
+        <v>8.86</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>7.79</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>6.75</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -653,231 +661,236 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>7.82</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>8.64</v>
+        <v>7.82</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>10.58</v>
+        <v>8.64</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>9.48</v>
+        <v>10.58</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>7.38</v>
+        <v>9.48</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>6.9</v>
+        <v>7.38</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>6.94</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>6.24</v>
+        <v>6.94</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>6.84</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>6.85</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>6.9</v>
+        <v>6.85</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>7.79</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>8.18</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>7.51</v>
+        <v>8.18</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>7.23</v>
+        <v>7.51</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>8.42</v>
+        <v>7.23</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>9.61</v>
+        <v>8.42</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>9.0500000000000007</v>
+        <v>9.61</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>9.26</v>
+        <v>9.0500000000000007</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>9.2200000000000006</v>
+        <v>9.26</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>9.3800000000000008</v>
+        <v>9.2200000000000006</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>9.1</v>
+        <v>9.3800000000000008</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>7.95</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>8.1199999999999992</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>9.75</v>
+        <v>8.1199999999999992</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>10.85</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>10.41</v>
+        <v>10.85</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>9.9600000000000009</v>
+        <v>10.41</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>9.61</v>
+        <v>9.9600000000000009</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>8.76</v>
+        <v>9.61</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>8.18</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>7.21</v>
+        <v>8.18</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>7.13</v>
+        <v>7.21</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>9.1</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>8.25</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>7.91</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>6.89</v>
+        <v>7.91</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>5.96</v>
+        <v>6.89</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>6.8</v>
+        <v>5.96</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>7.68</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>8.3800000000000008</v>
+        <v>7.68</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>8.52</v>
+        <v>8.3800000000000008</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>9.74</v>
+        <v>8.52</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>9.31</v>
+        <v>9.74</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>9.89</v>
+        <v>9.31</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
+        <v>9.89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
         <v>9.9600000000000009</v>
       </c>
     </row>

</xml_diff>